<commit_message>
- Correct WellEvent and LeaseID (tks Konstantin)
</commit_message>
<xml_diff>
--- a/calcroyalties/files/sample_data.xlsx
+++ b/calcroyalties/files/sample_data.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lshumlich/python/python-playground/calcroyalties/tempfiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lshumlich/python/python-playground/calcroyalties/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="520" yWindow="1620" windowWidth="28800" windowHeight="14940" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Well" sheetId="1" r:id="rId1"/>
     <sheet name="Lease" sheetId="2" r:id="rId2"/>
-    <sheet name="RoyaltyMaster" sheetId="3" r:id="rId3"/>
-    <sheet name="Monthly" sheetId="4" r:id="rId4"/>
-    <sheet name="Calc" sheetId="5" r:id="rId5"/>
-    <sheet name="ECONData" sheetId="8" r:id="rId6"/>
+    <sheet name="WellLeaseLink" sheetId="9" r:id="rId3"/>
+    <sheet name="RoyaltyMaster" sheetId="3" r:id="rId4"/>
+    <sheet name="Monthly" sheetId="4" r:id="rId5"/>
+    <sheet name="Calc" sheetId="5" r:id="rId6"/>
+    <sheet name="ECONData" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="147">
   <si>
     <t>ID</t>
   </si>
@@ -479,13 +480,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -508,10 +519,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,7 +806,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2096,7 +2113,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2369,6 +2386,703 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>9001</v>
+      </c>
+      <c r="F2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1001</v>
+      </c>
+      <c r="B3" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>9002</v>
+      </c>
+      <c r="F3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1002</v>
+      </c>
+      <c r="B4" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>9003</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1003</v>
+      </c>
+      <c r="B5" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>9004</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1004</v>
+      </c>
+      <c r="B6" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>9005</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1005</v>
+      </c>
+      <c r="B7" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>9006</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1006</v>
+      </c>
+      <c r="B8" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>9007</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1007</v>
+      </c>
+      <c r="B9" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>9008</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1008</v>
+      </c>
+      <c r="B10" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>9004</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1009</v>
+      </c>
+      <c r="B11" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>9005</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1010</v>
+      </c>
+      <c r="B12" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>9001</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1011</v>
+      </c>
+      <c r="B13" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>9002</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1012</v>
+      </c>
+      <c r="B14" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>9003</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1013</v>
+      </c>
+      <c r="B15" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>9004</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1014</v>
+      </c>
+      <c r="B16" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>9005</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1015</v>
+      </c>
+      <c r="B17" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>9001</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1016</v>
+      </c>
+      <c r="B18" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>9002</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1017</v>
+      </c>
+      <c r="B19" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>9003</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1018</v>
+      </c>
+      <c r="B20" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>9004</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1019</v>
+      </c>
+      <c r="B21" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21">
+        <v>9005</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1020</v>
+      </c>
+      <c r="B22" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22">
+        <v>9001</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1021</v>
+      </c>
+      <c r="B23" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>9002</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1022</v>
+      </c>
+      <c r="B24" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24">
+        <v>9003</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1023</v>
+      </c>
+      <c r="B25" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>9004</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1024</v>
+      </c>
+      <c r="B26" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>9005</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1025</v>
+      </c>
+      <c r="B27" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C27" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>9020</v>
+      </c>
+      <c r="F27">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1026</v>
+      </c>
+      <c r="B28" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C28" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>9006</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1027</v>
+      </c>
+      <c r="B29" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C29" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>9007</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1028</v>
+      </c>
+      <c r="B30" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C30" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30">
+        <v>9008</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1029</v>
+      </c>
+      <c r="B31" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C31" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>9009</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1030</v>
+      </c>
+      <c r="B32" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C32" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>9020</v>
+      </c>
+      <c r="F32">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1031</v>
+      </c>
+      <c r="B33" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C33" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33">
+        <v>9020</v>
+      </c>
+      <c r="F33">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1032</v>
+      </c>
+      <c r="B34" s="4">
+        <v>40969</v>
+      </c>
+      <c r="C34" s="4">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>9006</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -2696,7 +3410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
@@ -4422,7 +5136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC22"/>
   <sheetViews>
@@ -6315,11 +7029,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
- Get calc and worksheet working, revert back to wellID
</commit_message>
<xml_diff>
--- a/calcroyalties/files/sample_data.xlsx
+++ b/calcroyalties/files/sample_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lshumlich/python/python-playground/calcroyalties/tempfiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lshumlich/python/python-playground/calcroyalties/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14220" yWindow="2700" windowWidth="13180" windowHeight="13140" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Well" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="151">
   <si>
     <t>ID</t>
   </si>
@@ -315,18 +315,6 @@
   </si>
   <si>
     <t>dprod = 0.135135 = 100 / 740 is greater than 0.0 and less than or equal to 250.0 for a RoyRate of 2.0%</t>
-  </si>
-  <si>
-    <t>mprod = 100 is greater than 0.0 and less than or equal to 250.0 for a RoyRate of 2.0%</t>
-  </si>
-  <si>
-    <t>fixed for a RoyRate of 2.0%</t>
-  </si>
-  <si>
-    <t>dprod = 2.083333 = 100 / 48 is greater than 0.0 and less than or equal to 250.0 for a RoyRate of 2.0%</t>
-  </si>
-  <si>
-    <t>dprod = 4.166667 = 200 / 48 is greater than 0.0 and less than or equal to 250.0 for a RoyRate of 2.0%</t>
   </si>
   <si>
     <t>CharMonth</t>
@@ -853,13 +841,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -892,10 +880,10 @@
         <v>10</v>
       </c>
       <c r="O1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="P1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2164,10 +2152,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -2176,13 +2164,13 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" t="s">
         <v>145</v>
-      </c>
-      <c r="G1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H1" t="s">
-        <v>149</v>
       </c>
       <c r="I1" t="s">
         <v>31</v>
@@ -2443,10 +2431,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>56</v>
@@ -3143,10 +3131,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D1" t="s">
         <v>34</v>
@@ -3170,19 +3158,19 @@
         <v>40</v>
       </c>
       <c r="K1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L1" t="s">
         <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="O1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="P1" t="s">
         <v>31</v>
@@ -3521,7 +3509,7 @@
         <v>64</v>
       </c>
       <c r="M1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -5203,10 +5191,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE22"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5282,7 +5270,7 @@
         <v>85</v>
       </c>
       <c r="X1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Y1" t="s">
         <v>86</v>
@@ -5390,1711 +5378,6 @@
       </c>
       <c r="AE2" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>201501</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J3">
-        <v>14</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>2</v>
-      </c>
-      <c r="Q3">
-        <v>12</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>2680.44</v>
-      </c>
-      <c r="T3">
-        <v>446.74073199999998</v>
-      </c>
-      <c r="U3">
-        <v>3127.1807319999998</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>8629.43</v>
-      </c>
-      <c r="Z3">
-        <v>12</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>3127.1807319999998</v>
-      </c>
-      <c r="AC3">
-        <v>0.08</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>201501</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J4">
-        <v>14</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>2</v>
-      </c>
-      <c r="Q4">
-        <v>12</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>2680.44</v>
-      </c>
-      <c r="T4">
-        <v>446.74073199999998</v>
-      </c>
-      <c r="U4">
-        <v>3127.1807319999998</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>8629.43</v>
-      </c>
-      <c r="Z4">
-        <v>12</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>3127.1807319999998</v>
-      </c>
-      <c r="AC4">
-        <v>0.08</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>201501</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>27.11</v>
-      </c>
-      <c r="F5">
-        <v>626</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>221.123456</v>
-      </c>
-      <c r="J5">
-        <v>15.5</v>
-      </c>
-      <c r="K5">
-        <v>20.85</v>
-      </c>
-      <c r="L5">
-        <v>50</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5">
-        <v>15</v>
-      </c>
-      <c r="P5">
-        <v>0.5</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>3316.8518399999998</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>110.561728</v>
-      </c>
-      <c r="U5">
-        <v>3427.4135679999999</v>
-      </c>
-      <c r="V5">
-        <v>32.913552500000002</v>
-      </c>
-      <c r="W5">
-        <v>1.9135525</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>34.827105000000003</v>
-      </c>
-      <c r="AB5">
-        <v>3392.5864630000001</v>
-      </c>
-      <c r="AC5">
-        <v>0.08</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>201501</v>
-      </c>
-      <c r="C6">
-        <v>2001</v>
-      </c>
-      <c r="E6">
-        <v>27.11</v>
-      </c>
-      <c r="F6">
-        <v>626</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>221.123456</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>20.85</v>
-      </c>
-      <c r="L6">
-        <v>20.85</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>5.2125000000000004</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>1152.6060144</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>201501</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>9.3399999999999997E-2</v>
-      </c>
-      <c r="H7">
-        <v>2.34</v>
-      </c>
-      <c r="I7">
-        <v>221.123456</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>7</v>
-      </c>
-      <c r="L7">
-        <v>7</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>1.75</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>386.966048</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>201502</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>34.9</v>
-      </c>
-      <c r="F8">
-        <v>805</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J8">
-        <v>29.95825</v>
-      </c>
-      <c r="K8">
-        <v>26.85</v>
-      </c>
-      <c r="L8">
-        <v>26.85</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>2</v>
-      </c>
-      <c r="O8">
-        <v>28.058250000000001</v>
-      </c>
-      <c r="P8">
-        <v>1.9</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>6267.3815718195001</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>424.4036954</v>
-      </c>
-      <c r="U8">
-        <v>6691.7852672195004</v>
-      </c>
-      <c r="V8">
-        <v>63.614995753750001</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>63.614995753750001</v>
-      </c>
-      <c r="AB8">
-        <v>6628.1702714657504</v>
-      </c>
-      <c r="AC8">
-        <v>0.17</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>201503</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0.1237</v>
-      </c>
-      <c r="H9">
-        <v>3.09</v>
-      </c>
-      <c r="I9">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J9">
-        <v>10.352</v>
-      </c>
-      <c r="K9">
-        <v>9.2799999999999994</v>
-      </c>
-      <c r="L9">
-        <v>9.2799999999999994</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>2</v>
-      </c>
-      <c r="O9">
-        <v>8.3520000000000003</v>
-      </c>
-      <c r="P9">
-        <v>2</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>1865.5892968319999</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>446.74073199999998</v>
-      </c>
-      <c r="U9">
-        <v>2312.3300288320002</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>1.2780061599999999</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>1.2780061599999999</v>
-      </c>
-      <c r="AB9">
-        <v>2311.052022672</v>
-      </c>
-      <c r="AC9">
-        <v>5</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>201504</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>28.6</v>
-      </c>
-      <c r="F10">
-        <v>660</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>221.123456</v>
-      </c>
-      <c r="J10">
-        <v>15.5</v>
-      </c>
-      <c r="K10">
-        <v>22</v>
-      </c>
-      <c r="L10">
-        <v>50</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>2</v>
-      </c>
-      <c r="O10">
-        <v>15</v>
-      </c>
-      <c r="P10">
-        <v>0.5</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>3316.8518399999998</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>110.561728</v>
-      </c>
-      <c r="U10">
-        <v>3427.4135679999999</v>
-      </c>
-      <c r="V10">
-        <v>32.913552500000002</v>
-      </c>
-      <c r="W10">
-        <v>1.9135525</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-      <c r="Z10">
-        <v>0</v>
-      </c>
-      <c r="AA10">
-        <v>34.827105000000003</v>
-      </c>
-      <c r="AB10">
-        <v>3392.5864630000001</v>
-      </c>
-      <c r="AC10">
-        <v>0.33</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>201503</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>34.340000000000003</v>
-      </c>
-      <c r="F11">
-        <v>793</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J11">
-        <v>29.498449999999998</v>
-      </c>
-      <c r="K11">
-        <v>26.41</v>
-      </c>
-      <c r="L11">
-        <v>26.41</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>2</v>
-      </c>
-      <c r="O11">
-        <v>27.59845</v>
-      </c>
-      <c r="P11">
-        <v>1.9</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>6164.6758775326998</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>424.4036954</v>
-      </c>
-      <c r="U11">
-        <v>6589.0795729327001</v>
-      </c>
-      <c r="V11">
-        <v>62.638631144750001</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>62.638631144750001</v>
-      </c>
-      <c r="AB11">
-        <v>6526.4409417879497</v>
-      </c>
-      <c r="AC11">
-        <v>0.25</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>201503</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J12">
-        <v>14</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>2</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>2</v>
-      </c>
-      <c r="Q12">
-        <v>12</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>2680.44</v>
-      </c>
-      <c r="T12">
-        <v>446.74073199999998</v>
-      </c>
-      <c r="U12">
-        <v>3127.1807319999998</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <v>8629.43</v>
-      </c>
-      <c r="Z12">
-        <v>12</v>
-      </c>
-      <c r="AA12">
-        <v>0</v>
-      </c>
-      <c r="AB12">
-        <v>3127.1807319999998</v>
-      </c>
-      <c r="AC12">
-        <v>0.25</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>201503</v>
-      </c>
-      <c r="C13">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J13">
-        <v>14</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>2</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>2</v>
-      </c>
-      <c r="Q13">
-        <v>12</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>2680.44</v>
-      </c>
-      <c r="T13">
-        <v>446.74073199999998</v>
-      </c>
-      <c r="U13">
-        <v>3127.1807319999998</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="Y13">
-        <v>8629.43</v>
-      </c>
-      <c r="Z13">
-        <v>12</v>
-      </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
-      <c r="AB13">
-        <v>3127.1807319999998</v>
-      </c>
-      <c r="AC13">
-        <v>0.25</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>201504</v>
-      </c>
-      <c r="C14">
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J14">
-        <v>38.4</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>2</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>4</v>
-      </c>
-      <c r="Q14">
-        <v>34.4</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>7683.94</v>
-      </c>
-      <c r="T14">
-        <v>893.48146399999996</v>
-      </c>
-      <c r="U14">
-        <v>8577.4214639999991</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="Y14">
-        <v>16239.02</v>
-      </c>
-      <c r="Z14">
-        <v>34.4</v>
-      </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
-      <c r="AB14">
-        <v>8577.4214639999991</v>
-      </c>
-      <c r="AC14">
-        <v>0.33</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>201504</v>
-      </c>
-      <c r="C15">
-        <v>7</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J15">
-        <v>38.4</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>2</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>4</v>
-      </c>
-      <c r="Q15">
-        <v>34.4</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>7683.94</v>
-      </c>
-      <c r="T15">
-        <v>893.48146399999996</v>
-      </c>
-      <c r="U15">
-        <v>8577.4214639999991</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="Y15">
-        <v>16239.02</v>
-      </c>
-      <c r="Z15">
-        <v>34.4</v>
-      </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
-      <c r="AB15">
-        <v>8577.4214639999991</v>
-      </c>
-      <c r="AC15">
-        <v>0.33</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>201504</v>
-      </c>
-      <c r="C16">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J16">
-        <v>38.4</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>2</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>4</v>
-      </c>
-      <c r="Q16">
-        <v>34.4</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>7683.94</v>
-      </c>
-      <c r="T16">
-        <v>893.48146399999996</v>
-      </c>
-      <c r="U16">
-        <v>8577.4214639999991</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16">
-        <v>0</v>
-      </c>
-      <c r="Y16">
-        <v>16239.02</v>
-      </c>
-      <c r="Z16">
-        <v>34.4</v>
-      </c>
-      <c r="AA16">
-        <v>0</v>
-      </c>
-      <c r="AB16">
-        <v>8577.4214639999991</v>
-      </c>
-      <c r="AC16">
-        <v>0.33</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>201504</v>
-      </c>
-      <c r="C17">
-        <v>11</v>
-      </c>
-      <c r="E17">
-        <v>35.65</v>
-      </c>
-      <c r="F17">
-        <v>823</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>221.123456</v>
-      </c>
-      <c r="J17">
-        <v>62</v>
-      </c>
-      <c r="K17">
-        <v>27.42</v>
-      </c>
-      <c r="L17">
-        <v>50</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>2</v>
-      </c>
-      <c r="O17">
-        <v>60</v>
-      </c>
-      <c r="P17">
-        <v>2</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>13267.407359999999</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>442.24691200000001</v>
-      </c>
-      <c r="U17">
-        <v>13709.654272</v>
-      </c>
-      <c r="V17">
-        <v>131.65421000000001</v>
-      </c>
-      <c r="W17">
-        <v>7.65421</v>
-      </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <v>0</v>
-      </c>
-      <c r="AA17">
-        <v>139.30842000000001</v>
-      </c>
-      <c r="AB17">
-        <v>13570.345852</v>
-      </c>
-      <c r="AC17">
-        <v>5</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>201504</v>
-      </c>
-      <c r="C18">
-        <v>12</v>
-      </c>
-      <c r="E18">
-        <v>37.81</v>
-      </c>
-      <c r="F18">
-        <v>873</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J18">
-        <v>33.988</v>
-      </c>
-      <c r="K18">
-        <v>29.08</v>
-      </c>
-      <c r="L18">
-        <v>29.08</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>2</v>
-      </c>
-      <c r="O18">
-        <v>31.988</v>
-      </c>
-      <c r="P18">
-        <v>2</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>7145.1712676079997</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>446.74073199999998</v>
-      </c>
-      <c r="U18">
-        <v>7591.9119996079999</v>
-      </c>
-      <c r="V18">
-        <v>72.171988540000001</v>
-      </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
-      <c r="Z18">
-        <v>0</v>
-      </c>
-      <c r="AA18">
-        <v>72.171988540000001</v>
-      </c>
-      <c r="AB18">
-        <v>7519.7400110680001</v>
-      </c>
-      <c r="AC18">
-        <v>5</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>201504</v>
-      </c>
-      <c r="C19">
-        <v>14</v>
-      </c>
-      <c r="E19">
-        <v>28.6</v>
-      </c>
-      <c r="F19">
-        <v>660</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>22</v>
-      </c>
-      <c r="L19">
-        <v>22</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>27.5</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>6142.6850649999997</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
-      <c r="Z19">
-        <v>0</v>
-      </c>
-      <c r="AA19">
-        <v>0</v>
-      </c>
-      <c r="AB19">
-        <v>0</v>
-      </c>
-      <c r="AC19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>201504</v>
-      </c>
-      <c r="C20">
-        <v>15</v>
-      </c>
-      <c r="E20">
-        <v>40.58</v>
-      </c>
-      <c r="F20">
-        <v>937</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>31.21</v>
-      </c>
-      <c r="L20">
-        <v>31.21</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>26.528500000000001</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>5925.6807544310004</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="Y20">
-        <v>0</v>
-      </c>
-      <c r="Z20">
-        <v>0</v>
-      </c>
-      <c r="AA20">
-        <v>0</v>
-      </c>
-      <c r="AB20">
-        <v>0</v>
-      </c>
-      <c r="AC20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>201504</v>
-      </c>
-      <c r="C21">
-        <v>16</v>
-      </c>
-      <c r="E21">
-        <v>41.65</v>
-      </c>
-      <c r="F21">
-        <v>961</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>221.123456</v>
-      </c>
-      <c r="J21">
-        <v>62</v>
-      </c>
-      <c r="K21">
-        <v>32.04</v>
-      </c>
-      <c r="L21">
-        <v>50</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>2</v>
-      </c>
-      <c r="O21">
-        <v>60</v>
-      </c>
-      <c r="P21">
-        <v>2</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>13267.407359999999</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>442.24691200000001</v>
-      </c>
-      <c r="U21">
-        <v>13709.654272</v>
-      </c>
-      <c r="V21">
-        <v>131.65421000000001</v>
-      </c>
-      <c r="W21">
-        <v>7.65421</v>
-      </c>
-      <c r="Y21">
-        <v>0</v>
-      </c>
-      <c r="Z21">
-        <v>0</v>
-      </c>
-      <c r="AA21">
-        <v>139.30842000000001</v>
-      </c>
-      <c r="AB21">
-        <v>13570.345852</v>
-      </c>
-      <c r="AC21">
-        <v>5</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>201504</v>
-      </c>
-      <c r="C22">
-        <v>20</v>
-      </c>
-      <c r="E22">
-        <v>53.69</v>
-      </c>
-      <c r="F22">
-        <v>1239</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>223.37036599999999</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>41.3</v>
-      </c>
-      <c r="L22">
-        <v>41.3</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>35.104999999999997</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>7841.41669843</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22">
-        <v>0</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-      <c r="Z22">
-        <v>0</v>
-      </c>
-      <c r="AA22">
-        <v>0</v>
-      </c>
-      <c r="AB22">
-        <v>0</v>
-      </c>
-      <c r="AC22">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -7104,9 +5387,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF48"/>
+  <dimension ref="A1:AF59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -7115,97 +5400,97 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" t="s">
         <v>99</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>100</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>101</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>102</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>103</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>104</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>105</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>106</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>107</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>108</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>109</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>110</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>112</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>113</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>114</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>115</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>116</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>117</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
         <v>118</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>119</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>120</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>121</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>122</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>123</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>124</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
@@ -7213,7 +5498,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C2">
         <v>201111</v>
@@ -7311,7 +5596,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C3">
         <v>201112</v>
@@ -7409,7 +5694,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C4">
         <v>201201</v>
@@ -7507,7 +5792,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C5">
         <v>201202</v>
@@ -7605,7 +5890,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C6">
         <v>201203</v>
@@ -7703,7 +5988,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C7">
         <v>201204</v>
@@ -7801,7 +6086,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C8">
         <v>201205</v>
@@ -7899,7 +6184,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C9">
         <v>201206</v>
@@ -7997,7 +6282,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C10">
         <v>201207</v>
@@ -8095,7 +6380,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C11">
         <v>201208</v>
@@ -8193,7 +6478,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C12">
         <v>201209</v>
@@ -8291,7 +6576,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C13">
         <v>201210</v>
@@ -8389,7 +6674,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C14">
         <v>201211</v>
@@ -8487,7 +6772,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C15">
         <v>201212</v>
@@ -8585,7 +6870,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C16">
         <v>201301</v>
@@ -8683,7 +6968,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C17">
         <v>201302</v>
@@ -8781,7 +7066,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C18">
         <v>201303</v>
@@ -8879,7 +7164,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C19">
         <v>201304</v>
@@ -8977,7 +7262,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C20">
         <v>201305</v>
@@ -9075,7 +7360,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C21">
         <v>201306</v>
@@ -9173,7 +7458,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C22">
         <v>201307</v>
@@ -9271,7 +7556,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C23">
         <v>201308</v>
@@ -9369,7 +7654,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C24">
         <v>201309</v>
@@ -9467,7 +7752,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C25">
         <v>201310</v>
@@ -9565,7 +7850,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C26">
         <v>201311</v>
@@ -9663,7 +7948,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C27">
         <v>201312</v>
@@ -9761,7 +8046,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C28">
         <v>201401</v>
@@ -9859,7 +8144,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C29">
         <v>201402</v>
@@ -9957,7 +8242,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C30">
         <v>201403</v>
@@ -10055,7 +8340,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C31">
         <v>201404</v>
@@ -10153,7 +8438,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C32">
         <v>201405</v>
@@ -10251,7 +8536,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C33">
         <v>201406</v>
@@ -10349,7 +8634,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C34">
         <v>201407</v>
@@ -10447,7 +8732,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C35">
         <v>201408</v>
@@ -10545,7 +8830,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C36">
         <v>201409</v>
@@ -10643,7 +8928,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C37">
         <v>201410</v>
@@ -10741,7 +9026,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C38">
         <v>201411</v>
@@ -10839,7 +9124,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C39">
         <v>201412</v>
@@ -10937,7 +9222,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C40">
         <v>201501</v>
@@ -11035,7 +9320,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C41">
         <v>201502</v>
@@ -11133,7 +9418,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C42">
         <v>201503</v>
@@ -11231,7 +9516,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C43">
         <v>201504</v>
@@ -11329,7 +9614,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C44">
         <v>201505</v>
@@ -11427,7 +9712,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C45">
         <v>201506</v>
@@ -11525,7 +9810,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C46">
         <v>201507</v>
@@ -11623,7 +9908,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C47">
         <v>201508</v>
@@ -11721,7 +10006,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C48">
         <v>201509</v>
@@ -11812,6 +10097,1084 @@
       </c>
       <c r="AF48">
         <v>1214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49">
+        <v>201510</v>
+      </c>
+      <c r="D49">
+        <v>217</v>
+      </c>
+      <c r="E49">
+        <v>258</v>
+      </c>
+      <c r="F49">
+        <v>312</v>
+      </c>
+      <c r="G49">
+        <v>0.1066</v>
+      </c>
+      <c r="H49">
+        <v>2.67</v>
+      </c>
+      <c r="I49">
+        <v>26.39</v>
+      </c>
+      <c r="J49">
+        <v>1979</v>
+      </c>
+      <c r="K49">
+        <v>23.51</v>
+      </c>
+      <c r="L49">
+        <v>543</v>
+      </c>
+      <c r="M49">
+        <v>28.01</v>
+      </c>
+      <c r="N49">
+        <v>646</v>
+      </c>
+      <c r="O49">
+        <v>0.1172</v>
+      </c>
+      <c r="P49">
+        <v>2.93</v>
+      </c>
+      <c r="Q49">
+        <v>29.01</v>
+      </c>
+      <c r="R49">
+        <v>2176</v>
+      </c>
+      <c r="S49">
+        <v>34.159999999999997</v>
+      </c>
+      <c r="T49">
+        <v>788</v>
+      </c>
+      <c r="U49">
+        <v>39.83</v>
+      </c>
+      <c r="V49">
+        <v>919</v>
+      </c>
+      <c r="W49">
+        <v>0.12690000000000001</v>
+      </c>
+      <c r="X49">
+        <v>3.17</v>
+      </c>
+      <c r="Y49">
+        <v>31.4</v>
+      </c>
+      <c r="Z49">
+        <v>2355</v>
+      </c>
+      <c r="AA49">
+        <v>37.17</v>
+      </c>
+      <c r="AB49">
+        <v>858</v>
+      </c>
+      <c r="AC49">
+        <v>41.33</v>
+      </c>
+      <c r="AD49">
+        <v>954</v>
+      </c>
+      <c r="AE49">
+        <v>53.29</v>
+      </c>
+      <c r="AF49">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50">
+        <v>201511</v>
+      </c>
+      <c r="D50">
+        <v>174</v>
+      </c>
+      <c r="E50">
+        <v>221</v>
+      </c>
+      <c r="F50">
+        <v>292</v>
+      </c>
+      <c r="G50">
+        <v>9.0200000000000002E-2</v>
+      </c>
+      <c r="H50">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="I50">
+        <v>22.33</v>
+      </c>
+      <c r="J50">
+        <v>1675</v>
+      </c>
+      <c r="K50">
+        <v>21.29</v>
+      </c>
+      <c r="L50">
+        <v>491</v>
+      </c>
+      <c r="M50">
+        <v>26.9</v>
+      </c>
+      <c r="N50">
+        <v>621</v>
+      </c>
+      <c r="O50">
+        <v>0.10780000000000001</v>
+      </c>
+      <c r="P50">
+        <v>2.7</v>
+      </c>
+      <c r="Q50">
+        <v>26.69</v>
+      </c>
+      <c r="R50">
+        <v>2002</v>
+      </c>
+      <c r="S50">
+        <v>32.26</v>
+      </c>
+      <c r="T50">
+        <v>745</v>
+      </c>
+      <c r="U50">
+        <v>38.880000000000003</v>
+      </c>
+      <c r="V50">
+        <v>897</v>
+      </c>
+      <c r="W50">
+        <v>0.1237</v>
+      </c>
+      <c r="X50">
+        <v>3.09</v>
+      </c>
+      <c r="Y50">
+        <v>30.62</v>
+      </c>
+      <c r="Z50">
+        <v>2297</v>
+      </c>
+      <c r="AA50">
+        <v>36.6</v>
+      </c>
+      <c r="AB50">
+        <v>845</v>
+      </c>
+      <c r="AC50">
+        <v>41.05</v>
+      </c>
+      <c r="AD50">
+        <v>947</v>
+      </c>
+      <c r="AE50">
+        <v>52.93</v>
+      </c>
+      <c r="AF50">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51">
+        <v>201512</v>
+      </c>
+      <c r="D51">
+        <v>131</v>
+      </c>
+      <c r="E51">
+        <v>183</v>
+      </c>
+      <c r="F51">
+        <v>245</v>
+      </c>
+      <c r="G51">
+        <v>6.3E-2</v>
+      </c>
+      <c r="H51">
+        <v>1.57</v>
+      </c>
+      <c r="I51">
+        <v>15.59</v>
+      </c>
+      <c r="J51">
+        <v>1169</v>
+      </c>
+      <c r="K51">
+        <v>17.61</v>
+      </c>
+      <c r="L51">
+        <v>406</v>
+      </c>
+      <c r="M51">
+        <v>25.06</v>
+      </c>
+      <c r="N51">
+        <v>578</v>
+      </c>
+      <c r="O51">
+        <v>9.4299999999999995E-2</v>
+      </c>
+      <c r="P51">
+        <v>2.36</v>
+      </c>
+      <c r="Q51">
+        <v>23.34</v>
+      </c>
+      <c r="R51">
+        <v>1751</v>
+      </c>
+      <c r="S51">
+        <v>29.52</v>
+      </c>
+      <c r="T51">
+        <v>681</v>
+      </c>
+      <c r="U51">
+        <v>37.51</v>
+      </c>
+      <c r="V51">
+        <v>866</v>
+      </c>
+      <c r="W51">
+        <v>0.1142</v>
+      </c>
+      <c r="X51">
+        <v>2.86</v>
+      </c>
+      <c r="Y51">
+        <v>28.27</v>
+      </c>
+      <c r="Z51">
+        <v>2120</v>
+      </c>
+      <c r="AA51">
+        <v>34.89</v>
+      </c>
+      <c r="AB51">
+        <v>805</v>
+      </c>
+      <c r="AC51">
+        <v>40.19</v>
+      </c>
+      <c r="AD51">
+        <v>928</v>
+      </c>
+      <c r="AE51">
+        <v>51.87</v>
+      </c>
+      <c r="AF51">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52">
+        <v>201601</v>
+      </c>
+      <c r="D52">
+        <v>88</v>
+      </c>
+      <c r="E52">
+        <v>151</v>
+      </c>
+      <c r="F52">
+        <v>197</v>
+      </c>
+      <c r="G52">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="H52">
+        <v>0.72</v>
+      </c>
+      <c r="I52">
+        <v>7.14</v>
+      </c>
+      <c r="J52">
+        <v>536</v>
+      </c>
+      <c r="K52">
+        <v>13</v>
+      </c>
+      <c r="L52">
+        <v>300</v>
+      </c>
+      <c r="M52">
+        <v>21.42</v>
+      </c>
+      <c r="N52">
+        <v>494</v>
+      </c>
+      <c r="O52">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="P52">
+        <v>1.94</v>
+      </c>
+      <c r="Q52">
+        <v>19.2</v>
+      </c>
+      <c r="R52">
+        <v>1440</v>
+      </c>
+      <c r="S52">
+        <v>26.13</v>
+      </c>
+      <c r="T52">
+        <v>603</v>
+      </c>
+      <c r="U52">
+        <v>35.81</v>
+      </c>
+      <c r="V52">
+        <v>826</v>
+      </c>
+      <c r="W52">
+        <v>9.9900000000000003E-2</v>
+      </c>
+      <c r="X52">
+        <v>2.5</v>
+      </c>
+      <c r="Y52">
+        <v>24.72</v>
+      </c>
+      <c r="Z52">
+        <v>1854</v>
+      </c>
+      <c r="AA52">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="AB52">
+        <v>745</v>
+      </c>
+      <c r="AC52">
+        <v>38.9</v>
+      </c>
+      <c r="AD52">
+        <v>898</v>
+      </c>
+      <c r="AE52">
+        <v>50.25</v>
+      </c>
+      <c r="AF52">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53">
+        <v>201602</v>
+      </c>
+      <c r="D53">
+        <v>76</v>
+      </c>
+      <c r="E53">
+        <v>132</v>
+      </c>
+      <c r="F53">
+        <v>181</v>
+      </c>
+      <c r="G53">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="H53">
+        <v>0.72</v>
+      </c>
+      <c r="I53">
+        <v>7.14</v>
+      </c>
+      <c r="J53">
+        <v>536</v>
+      </c>
+      <c r="K53">
+        <v>13</v>
+      </c>
+      <c r="L53">
+        <v>300</v>
+      </c>
+      <c r="M53">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="N53">
+        <v>454</v>
+      </c>
+      <c r="O53">
+        <v>6.3799999999999996E-2</v>
+      </c>
+      <c r="P53">
+        <v>1.6</v>
+      </c>
+      <c r="Q53">
+        <v>15.8</v>
+      </c>
+      <c r="R53">
+        <v>1185</v>
+      </c>
+      <c r="S53">
+        <v>23.34</v>
+      </c>
+      <c r="T53">
+        <v>539</v>
+      </c>
+      <c r="U53">
+        <v>34.42</v>
+      </c>
+      <c r="V53">
+        <v>794</v>
+      </c>
+      <c r="W53">
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="X53">
+        <v>2.34</v>
+      </c>
+      <c r="Y53">
+        <v>23.12</v>
+      </c>
+      <c r="Z53">
+        <v>1734</v>
+      </c>
+      <c r="AA53">
+        <v>31.14</v>
+      </c>
+      <c r="AB53">
+        <v>719</v>
+      </c>
+      <c r="AC53">
+        <v>38.32</v>
+      </c>
+      <c r="AD53">
+        <v>884</v>
+      </c>
+      <c r="AE53">
+        <v>49.52</v>
+      </c>
+      <c r="AF53">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>128</v>
+      </c>
+      <c r="C54">
+        <v>201603</v>
+      </c>
+      <c r="D54">
+        <v>137</v>
+      </c>
+      <c r="E54">
+        <v>186</v>
+      </c>
+      <c r="F54">
+        <v>238</v>
+      </c>
+      <c r="G54">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="H54">
+        <v>1.69</v>
+      </c>
+      <c r="I54">
+        <v>16.78</v>
+      </c>
+      <c r="J54">
+        <v>1259</v>
+      </c>
+      <c r="K54">
+        <v>18.27</v>
+      </c>
+      <c r="L54">
+        <v>422</v>
+      </c>
+      <c r="M54">
+        <v>25.38</v>
+      </c>
+      <c r="N54">
+        <v>586</v>
+      </c>
+      <c r="O54">
+        <v>9.5600000000000004E-2</v>
+      </c>
+      <c r="P54">
+        <v>2.39</v>
+      </c>
+      <c r="Q54">
+        <v>23.65</v>
+      </c>
+      <c r="R54">
+        <v>1774</v>
+      </c>
+      <c r="S54">
+        <v>29.77</v>
+      </c>
+      <c r="T54">
+        <v>687</v>
+      </c>
+      <c r="U54">
+        <v>37.64</v>
+      </c>
+      <c r="V54">
+        <v>869</v>
+      </c>
+      <c r="W54">
+        <v>0.1125</v>
+      </c>
+      <c r="X54">
+        <v>2.81</v>
+      </c>
+      <c r="Y54">
+        <v>27.85</v>
+      </c>
+      <c r="Z54">
+        <v>2089</v>
+      </c>
+      <c r="AA54">
+        <v>34.58</v>
+      </c>
+      <c r="AB54">
+        <v>798</v>
+      </c>
+      <c r="AC54">
+        <v>40.04</v>
+      </c>
+      <c r="AD54">
+        <v>924</v>
+      </c>
+      <c r="AE54">
+        <v>51.67</v>
+      </c>
+      <c r="AF54">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55">
+        <v>201604</v>
+      </c>
+      <c r="D55">
+        <v>169</v>
+      </c>
+      <c r="E55">
+        <v>216</v>
+      </c>
+      <c r="F55">
+        <v>263</v>
+      </c>
+      <c r="G55">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="H55">
+        <v>2.19</v>
+      </c>
+      <c r="I55">
+        <v>21.72</v>
+      </c>
+      <c r="J55">
+        <v>1629</v>
+      </c>
+      <c r="K55">
+        <v>20.96</v>
+      </c>
+      <c r="L55">
+        <v>484</v>
+      </c>
+      <c r="M55">
+        <v>26.73</v>
+      </c>
+      <c r="N55">
+        <v>617</v>
+      </c>
+      <c r="O55">
+        <v>0.10639999999999999</v>
+      </c>
+      <c r="P55">
+        <v>2.66</v>
+      </c>
+      <c r="Q55">
+        <v>26.32</v>
+      </c>
+      <c r="R55">
+        <v>1974</v>
+      </c>
+      <c r="S55">
+        <v>31.96</v>
+      </c>
+      <c r="T55">
+        <v>738</v>
+      </c>
+      <c r="U55">
+        <v>38.729999999999997</v>
+      </c>
+      <c r="V55">
+        <v>894</v>
+      </c>
+      <c r="W55">
+        <v>0.1183</v>
+      </c>
+      <c r="X55">
+        <v>2.96</v>
+      </c>
+      <c r="Y55">
+        <v>29.27</v>
+      </c>
+      <c r="Z55">
+        <v>2195</v>
+      </c>
+      <c r="AA55">
+        <v>35.61</v>
+      </c>
+      <c r="AB55">
+        <v>822</v>
+      </c>
+      <c r="AC55">
+        <v>40.56</v>
+      </c>
+      <c r="AD55">
+        <v>936</v>
+      </c>
+      <c r="AE55">
+        <v>52.32</v>
+      </c>
+      <c r="AF55">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56">
+        <v>201605</v>
+      </c>
+      <c r="D56">
+        <v>207</v>
+      </c>
+      <c r="E56">
+        <v>255</v>
+      </c>
+      <c r="F56">
+        <v>300</v>
+      </c>
+      <c r="G56">
+        <v>0.10340000000000001</v>
+      </c>
+      <c r="H56">
+        <v>2.59</v>
+      </c>
+      <c r="I56">
+        <v>25.6</v>
+      </c>
+      <c r="J56">
+        <v>1920</v>
+      </c>
+      <c r="K56">
+        <v>23.08</v>
+      </c>
+      <c r="L56">
+        <v>533</v>
+      </c>
+      <c r="M56">
+        <v>27.79</v>
+      </c>
+      <c r="N56">
+        <v>641</v>
+      </c>
+      <c r="O56">
+        <v>0.1166</v>
+      </c>
+      <c r="P56">
+        <v>2.91</v>
+      </c>
+      <c r="Q56">
+        <v>28.85</v>
+      </c>
+      <c r="R56">
+        <v>2164</v>
+      </c>
+      <c r="S56">
+        <v>34.03</v>
+      </c>
+      <c r="T56">
+        <v>785</v>
+      </c>
+      <c r="U56">
+        <v>39.76</v>
+      </c>
+      <c r="V56">
+        <v>918</v>
+      </c>
+      <c r="W56">
+        <v>0.12509999999999999</v>
+      </c>
+      <c r="X56">
+        <v>3.13</v>
+      </c>
+      <c r="Y56">
+        <v>30.95</v>
+      </c>
+      <c r="Z56">
+        <v>2321</v>
+      </c>
+      <c r="AA56">
+        <v>36.83</v>
+      </c>
+      <c r="AB56">
+        <v>850</v>
+      </c>
+      <c r="AC56">
+        <v>41.17</v>
+      </c>
+      <c r="AD56">
+        <v>950</v>
+      </c>
+      <c r="AE56">
+        <v>53.08</v>
+      </c>
+      <c r="AF56">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>131</v>
+      </c>
+      <c r="C57">
+        <v>201606</v>
+      </c>
+      <c r="D57">
+        <v>252</v>
+      </c>
+      <c r="E57">
+        <v>285</v>
+      </c>
+      <c r="F57">
+        <v>330</v>
+      </c>
+      <c r="G57">
+        <v>0.1159</v>
+      </c>
+      <c r="H57">
+        <v>2.9</v>
+      </c>
+      <c r="I57">
+        <v>28.68</v>
+      </c>
+      <c r="J57">
+        <v>2151</v>
+      </c>
+      <c r="K57">
+        <v>24.76</v>
+      </c>
+      <c r="L57">
+        <v>571</v>
+      </c>
+      <c r="M57">
+        <v>28.63</v>
+      </c>
+      <c r="N57">
+        <v>661</v>
+      </c>
+      <c r="O57">
+        <v>0.1225</v>
+      </c>
+      <c r="P57">
+        <v>3.06</v>
+      </c>
+      <c r="Q57">
+        <v>30.32</v>
+      </c>
+      <c r="R57">
+        <v>2274</v>
+      </c>
+      <c r="S57">
+        <v>35.24</v>
+      </c>
+      <c r="T57">
+        <v>813</v>
+      </c>
+      <c r="U57">
+        <v>40.369999999999997</v>
+      </c>
+      <c r="V57">
+        <v>932</v>
+      </c>
+      <c r="W57">
+        <v>0.12939999999999999</v>
+      </c>
+      <c r="X57">
+        <v>3.24</v>
+      </c>
+      <c r="Y57">
+        <v>32.03</v>
+      </c>
+      <c r="Z57">
+        <v>2402</v>
+      </c>
+      <c r="AA57">
+        <v>37.619999999999997</v>
+      </c>
+      <c r="AB57">
+        <v>868</v>
+      </c>
+      <c r="AC57">
+        <v>41.56</v>
+      </c>
+      <c r="AD57">
+        <v>959</v>
+      </c>
+      <c r="AE57">
+        <v>53.58</v>
+      </c>
+      <c r="AF57">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58">
+        <v>201607</v>
+      </c>
+      <c r="D58">
+        <v>226</v>
+      </c>
+      <c r="E58">
+        <v>259</v>
+      </c>
+      <c r="F58">
+        <v>311</v>
+      </c>
+      <c r="G58">
+        <v>0.10929999999999999</v>
+      </c>
+      <c r="H58">
+        <v>2.73</v>
+      </c>
+      <c r="I58">
+        <v>27.05</v>
+      </c>
+      <c r="J58">
+        <v>2029</v>
+      </c>
+      <c r="K58">
+        <v>23.87</v>
+      </c>
+      <c r="L58">
+        <v>551</v>
+      </c>
+      <c r="M58">
+        <v>28.19</v>
+      </c>
+      <c r="N58">
+        <v>651</v>
+      </c>
+      <c r="O58">
+        <v>0.1174</v>
+      </c>
+      <c r="P58">
+        <v>2.94</v>
+      </c>
+      <c r="Q58">
+        <v>29.06</v>
+      </c>
+      <c r="R58">
+        <v>2180</v>
+      </c>
+      <c r="S58">
+        <v>34.21</v>
+      </c>
+      <c r="T58">
+        <v>790</v>
+      </c>
+      <c r="U58">
+        <v>39.85</v>
+      </c>
+      <c r="V58">
+        <v>920</v>
+      </c>
+      <c r="W58">
+        <v>0.1268</v>
+      </c>
+      <c r="X58">
+        <v>3.17</v>
+      </c>
+      <c r="Y58">
+        <v>31.37</v>
+      </c>
+      <c r="Z58">
+        <v>2353</v>
+      </c>
+      <c r="AA58">
+        <v>37.14</v>
+      </c>
+      <c r="AB58">
+        <v>857</v>
+      </c>
+      <c r="AC58">
+        <v>41.32</v>
+      </c>
+      <c r="AD58">
+        <v>954</v>
+      </c>
+      <c r="AE58">
+        <v>53.27</v>
+      </c>
+      <c r="AF58">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59">
+        <v>201608</v>
+      </c>
+      <c r="D59">
+        <v>209</v>
+      </c>
+      <c r="E59">
+        <v>243</v>
+      </c>
+      <c r="F59">
+        <v>296</v>
+      </c>
+      <c r="G59">
+        <v>0.1041</v>
+      </c>
+      <c r="H59">
+        <v>2.6</v>
+      </c>
+      <c r="I59">
+        <v>25.76</v>
+      </c>
+      <c r="J59">
+        <v>1932</v>
+      </c>
+      <c r="K59">
+        <v>23.17</v>
+      </c>
+      <c r="L59">
+        <v>535</v>
+      </c>
+      <c r="M59">
+        <v>27.83</v>
+      </c>
+      <c r="N59">
+        <v>642</v>
+      </c>
+      <c r="O59">
+        <v>0.1137</v>
+      </c>
+      <c r="P59">
+        <v>2.84</v>
+      </c>
+      <c r="Q59">
+        <v>28.15</v>
+      </c>
+      <c r="R59">
+        <v>2111</v>
+      </c>
+      <c r="S59">
+        <v>33.46</v>
+      </c>
+      <c r="T59">
+        <v>772</v>
+      </c>
+      <c r="U59">
+        <v>39.479999999999997</v>
+      </c>
+      <c r="V59">
+        <v>911</v>
+      </c>
+      <c r="W59">
+        <v>0.1244</v>
+      </c>
+      <c r="X59">
+        <v>3.11</v>
+      </c>
+      <c r="Y59">
+        <v>30.79</v>
+      </c>
+      <c r="Z59">
+        <v>2309</v>
+      </c>
+      <c r="AA59">
+        <v>36.72</v>
+      </c>
+      <c r="AB59">
+        <v>847</v>
+      </c>
+      <c r="AC59">
+        <v>41.11</v>
+      </c>
+      <c r="AD59">
+        <v>949</v>
+      </c>
+      <c r="AE59">
+        <v>53.01</v>
+      </c>
+      <c r="AF59">
+        <v>1223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Change Rates and Percentages to be base 1
</commit_message>
<xml_diff>
--- a/calcroyalties/files/sample_data.xlsx
+++ b/calcroyalties/files/sample_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lshumlich/python/python-playground/calcroyalties/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lshumlich/python/python-playground/calcroyalties/tempfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-160" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Well" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="151">
   <si>
     <t>ID</t>
   </si>
@@ -146,9 +146,6 @@
     <t>CrownMultiplier</t>
   </si>
   <si>
-    <t>MinRoyalty</t>
-  </si>
-  <si>
     <t>ValuationMethod</t>
   </si>
   <si>
@@ -486,6 +483,9 @@
   </si>
   <si>
     <t>RoyaltyGCA</t>
+  </si>
+  <si>
+    <t>MinRoyaltyDollar</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,14 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -534,20 +541,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -822,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,21 +844,22 @@
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
         <v>138</v>
       </c>
-      <c r="C1" t="s">
-        <v>139</v>
-      </c>
       <c r="D1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -856,37 +868,28 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
         <v>143</v>
       </c>
-      <c r="P1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -906,31 +909,22 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2">
-        <v>9001</v>
-      </c>
-      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>41974</v>
+      </c>
       <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0.25</v>
-      </c>
-      <c r="M2" s="1">
-        <v>41974</v>
-      </c>
-      <c r="N2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -950,31 +944,22 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3">
-        <v>9002</v>
-      </c>
-      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>41974</v>
+      </c>
       <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0.95</v>
-      </c>
-      <c r="M3" s="1">
-        <v>41974</v>
-      </c>
-      <c r="N3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -994,25 +979,16 @@
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4">
-        <v>9003</v>
-      </c>
-      <c r="I4" t="s">
         <v>21</v>
       </c>
-      <c r="J4" t="s">
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="K4">
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1032,25 +1008,16 @@
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5">
-        <v>9004</v>
-      </c>
-      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" t="s">
+      <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="K5">
+      <c r="I5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1070,22 +1037,13 @@
         <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6">
-        <v>9005</v>
-      </c>
-      <c r="I6" t="s">
         <v>27</v>
       </c>
-      <c r="K6">
+      <c r="I6">
         <v>0</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1105,28 +1063,19 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7">
-        <v>9006</v>
-      </c>
-      <c r="I7" t="s">
         <v>21</v>
       </c>
-      <c r="J7" t="s">
+      <c r="H7" t="s">
         <v>16</v>
       </c>
-      <c r="K7">
+      <c r="I7">
         <v>0</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7" s="1">
+      <c r="J7" s="1">
         <v>41974</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1146,28 +1095,19 @@
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8">
-        <v>9007</v>
-      </c>
-      <c r="I8" t="s">
         <v>21</v>
       </c>
-      <c r="J8" t="s">
+      <c r="H8" t="s">
         <v>19</v>
       </c>
-      <c r="K8">
+      <c r="I8">
         <v>0</v>
       </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8" s="1">
+      <c r="J8" s="1">
         <v>41974</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1187,28 +1127,19 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9">
-        <v>9008</v>
-      </c>
-      <c r="I9" t="s">
         <v>21</v>
       </c>
-      <c r="J9" t="s">
+      <c r="H9" t="s">
         <v>22</v>
       </c>
-      <c r="K9">
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9" s="1">
+      <c r="J9" s="1">
         <v>41974</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1228,25 +1159,16 @@
         <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10">
-        <v>9004</v>
-      </c>
-      <c r="I10" t="s">
         <v>21</v>
       </c>
-      <c r="J10" t="s">
+      <c r="H10" t="s">
         <v>29</v>
       </c>
-      <c r="K10">
+      <c r="I10">
         <v>0</v>
       </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1266,25 +1188,16 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11">
-        <v>9005</v>
-      </c>
-      <c r="I11" t="s">
         <v>18</v>
       </c>
-      <c r="J11" t="s">
+      <c r="H11" t="s">
         <v>16</v>
       </c>
-      <c r="K11">
+      <c r="I11">
         <v>0</v>
       </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1304,25 +1217,16 @@
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12">
-        <v>9001</v>
-      </c>
-      <c r="I12" t="s">
         <v>18</v>
       </c>
-      <c r="J12" t="s">
+      <c r="H12" t="s">
         <v>19</v>
       </c>
-      <c r="K12">
+      <c r="I12">
         <v>0</v>
       </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1342,25 +1246,16 @@
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13">
-        <v>9002</v>
-      </c>
-      <c r="I13" t="s">
         <v>18</v>
       </c>
-      <c r="J13" t="s">
+      <c r="H13" t="s">
         <v>22</v>
       </c>
-      <c r="K13">
+      <c r="I13">
         <v>0</v>
       </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1380,25 +1275,16 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14">
-        <v>9003</v>
-      </c>
-      <c r="I14" t="s">
         <v>18</v>
       </c>
-      <c r="J14" t="s">
+      <c r="H14" t="s">
         <v>29</v>
       </c>
-      <c r="K14">
+      <c r="I14">
         <v>0</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1418,25 +1304,16 @@
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15">
-        <v>9004</v>
-      </c>
-      <c r="I15" t="s">
         <v>15</v>
       </c>
-      <c r="J15" t="s">
+      <c r="H15" t="s">
         <v>16</v>
       </c>
-      <c r="K15">
+      <c r="I15">
         <v>0</v>
       </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1456,25 +1333,16 @@
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16">
-        <v>9005</v>
-      </c>
-      <c r="I16" t="s">
         <v>15</v>
       </c>
-      <c r="J16" t="s">
+      <c r="H16" t="s">
         <v>19</v>
       </c>
-      <c r="K16">
+      <c r="I16">
         <v>0</v>
       </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1494,25 +1362,16 @@
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17">
-        <v>9001</v>
-      </c>
-      <c r="I17" t="s">
         <v>15</v>
       </c>
-      <c r="J17" t="s">
+      <c r="H17" t="s">
         <v>22</v>
       </c>
-      <c r="K17">
+      <c r="I17">
         <v>0</v>
       </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1532,25 +1391,16 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18">
-        <v>9002</v>
-      </c>
-      <c r="I18" t="s">
         <v>15</v>
       </c>
-      <c r="J18" t="s">
+      <c r="H18" t="s">
         <v>29</v>
       </c>
-      <c r="K18">
+      <c r="I18">
         <v>0</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1570,25 +1420,16 @@
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19">
-        <v>9003</v>
-      </c>
-      <c r="I19" t="s">
         <v>24</v>
       </c>
-      <c r="J19" t="s">
+      <c r="H19" t="s">
         <v>16</v>
       </c>
-      <c r="K19">
+      <c r="I19">
         <v>0</v>
       </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1608,25 +1449,16 @@
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20">
-        <v>9004</v>
-      </c>
-      <c r="I20" t="s">
         <v>24</v>
       </c>
-      <c r="J20" t="s">
+      <c r="H20" t="s">
         <v>19</v>
       </c>
-      <c r="K20">
+      <c r="I20">
         <v>0</v>
       </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1646,25 +1478,16 @@
         <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21">
-        <v>9005</v>
-      </c>
-      <c r="I21" t="s">
         <v>24</v>
       </c>
-      <c r="J21" t="s">
+      <c r="H21" t="s">
         <v>22</v>
       </c>
-      <c r="K21">
+      <c r="I21">
         <v>0</v>
       </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1684,25 +1507,16 @@
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22">
-        <v>9001</v>
-      </c>
-      <c r="I22" t="s">
         <v>24</v>
       </c>
-      <c r="J22" t="s">
+      <c r="H22" t="s">
         <v>29</v>
       </c>
-      <c r="K22">
+      <c r="I22">
         <v>0</v>
       </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1722,25 +1536,16 @@
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23">
-        <v>9002</v>
-      </c>
-      <c r="I23" t="s">
         <v>30</v>
       </c>
-      <c r="J23" t="s">
+      <c r="H23" t="s">
         <v>16</v>
       </c>
-      <c r="K23">
+      <c r="I23">
         <v>0</v>
       </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1760,25 +1565,16 @@
         <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24">
-        <v>9003</v>
-      </c>
-      <c r="I24" t="s">
         <v>30</v>
       </c>
-      <c r="J24" t="s">
+      <c r="H24" t="s">
         <v>19</v>
       </c>
-      <c r="K24">
+      <c r="I24">
         <v>0</v>
       </c>
-      <c r="L24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1798,25 +1594,16 @@
         <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25">
-        <v>9004</v>
-      </c>
-      <c r="I25" t="s">
         <v>30</v>
       </c>
-      <c r="J25" t="s">
+      <c r="H25" t="s">
         <v>22</v>
       </c>
-      <c r="K25">
+      <c r="I25">
         <v>0</v>
       </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1836,25 +1623,16 @@
         <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26">
-        <v>9005</v>
-      </c>
-      <c r="I26" t="s">
         <v>30</v>
       </c>
-      <c r="J26" t="s">
+      <c r="H26" t="s">
         <v>29</v>
       </c>
-      <c r="K26">
+      <c r="I26">
         <v>0</v>
       </c>
-      <c r="L26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>30</v>
       </c>
@@ -1874,25 +1652,16 @@
         <v>13</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27">
-        <v>9020</v>
-      </c>
-      <c r="I27" t="s">
         <v>21</v>
       </c>
-      <c r="J27" t="s">
+      <c r="H27" t="s">
         <v>16</v>
       </c>
-      <c r="K27">
+      <c r="I27">
         <v>0</v>
       </c>
-      <c r="L27">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>31</v>
       </c>
@@ -1911,20 +1680,11 @@
       <c r="F28" t="s">
         <v>13</v>
       </c>
-      <c r="G28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28">
-        <v>9006</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
-      </c>
-      <c r="M28" s="1">
+      <c r="J28" s="1">
         <v>40513</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>32</v>
       </c>
@@ -1943,20 +1703,11 @@
       <c r="F29" t="s">
         <v>13</v>
       </c>
-      <c r="G29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29">
-        <v>9007</v>
-      </c>
-      <c r="L29">
-        <v>1</v>
-      </c>
-      <c r="M29" s="1">
+      <c r="J29" s="1">
         <v>40513</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>33</v>
       </c>
@@ -1975,20 +1726,11 @@
       <c r="F30" t="s">
         <v>13</v>
       </c>
-      <c r="G30" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30">
-        <v>9008</v>
-      </c>
-      <c r="L30">
-        <v>1</v>
-      </c>
-      <c r="M30" s="1">
+      <c r="J30" s="1">
         <v>41974</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1000</v>
       </c>
@@ -2007,20 +1749,11 @@
       <c r="F31" t="s">
         <v>13</v>
       </c>
-      <c r="G31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31">
-        <v>9009</v>
-      </c>
-      <c r="L31">
-        <v>1</v>
-      </c>
-      <c r="M31" s="1">
+      <c r="J31" s="1">
         <v>41609</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2000</v>
       </c>
@@ -2040,25 +1773,16 @@
         <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32">
-        <v>9020</v>
-      </c>
-      <c r="I32" t="s">
         <v>21</v>
       </c>
-      <c r="J32" t="s">
+      <c r="H32" t="s">
         <v>16</v>
       </c>
-      <c r="K32">
+      <c r="I32">
         <v>0</v>
       </c>
-      <c r="L32">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2001</v>
       </c>
@@ -2078,25 +1802,16 @@
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33">
-        <v>9020</v>
-      </c>
-      <c r="I33" t="s">
         <v>15</v>
       </c>
-      <c r="J33" t="s">
+      <c r="H33" t="s">
         <v>16</v>
       </c>
-      <c r="K33">
+      <c r="I33">
         <v>0</v>
       </c>
-      <c r="L33">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3000</v>
       </c>
@@ -2115,16 +1830,7 @@
       <c r="F34" t="s">
         <v>13</v>
       </c>
-      <c r="G34" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34">
-        <v>9006</v>
-      </c>
-      <c r="L34">
-        <v>1</v>
-      </c>
-      <c r="M34" s="1">
+      <c r="J34" s="1">
         <v>40513</v>
       </c>
     </row>
@@ -2152,10 +1858,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
         <v>138</v>
-      </c>
-      <c r="C1" t="s">
-        <v>139</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -2164,13 +1870,13 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I1" t="s">
         <v>31</v>
@@ -2431,13 +2137,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -3107,7 +2813,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -3118,12 +2824,18 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -3131,10 +2843,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
         <v>138</v>
-      </c>
-      <c r="C1" t="s">
-        <v>139</v>
       </c>
       <c r="D1" t="s">
         <v>34</v>
@@ -3155,22 +2867,22 @@
         <v>39</v>
       </c>
       <c r="J1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M1" t="s">
         <v>146</v>
-      </c>
-      <c r="L1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" t="s">
-        <v>142</v>
       </c>
       <c r="N1" t="s">
         <v>147</v>
       </c>
       <c r="O1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="P1" t="s">
         <v>31</v>
@@ -3187,28 +2899,31 @@
         <v>2958465</v>
       </c>
       <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="G2" t="s">
         <v>43</v>
-      </c>
-      <c r="F2">
-        <v>1.2</v>
-      </c>
-      <c r="G2">
-        <v>50</v>
       </c>
       <c r="H2" t="s">
         <v>44</v>
       </c>
       <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" t="s">
-        <v>46</v>
+      <c r="M2">
+        <v>0.35</v>
+      </c>
+      <c r="O2" s="5">
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -3222,25 +2937,25 @@
         <v>2958465</v>
       </c>
       <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
         <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
       </c>
       <c r="F3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3">
         <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -3254,22 +2969,22 @@
         <v>2958465</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4">
         <v>0.9</v>
       </c>
-      <c r="H4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" t="s">
-        <v>50</v>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -3283,22 +2998,22 @@
         <v>2958465</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5">
         <v>1.25</v>
       </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -3312,16 +3027,19 @@
         <v>2958465</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>0.85</v>
       </c>
-      <c r="H6" t="s">
-        <v>47</v>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6">
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -3335,19 +3053,19 @@
         <v>2958465</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
         <v>47</v>
-      </c>
-      <c r="L7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -3361,19 +3079,19 @@
         <v>2958465</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" t="s">
         <v>47</v>
-      </c>
-      <c r="L8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -3387,19 +3105,19 @@
         <v>2958465</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" t="s">
         <v>47</v>
-      </c>
-      <c r="L9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -3413,16 +3131,16 @@
         <v>2958465</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
-        <v>44</v>
+      <c r="G10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -3436,19 +3154,19 @@
         <v>2958465</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11">
         <v>1.2</v>
       </c>
-      <c r="H11" t="s">
-        <v>44</v>
+      <c r="G11" t="s">
+        <v>43</v>
       </c>
       <c r="P11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -3476,40 +3194,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>62</v>
       </c>
-      <c r="J1" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>63</v>
       </c>
-      <c r="L1" t="s">
-        <v>64</v>
-      </c>
       <c r="M1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -4096,7 +3814,7 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17">
         <v>6</v>
@@ -4134,7 +3852,7 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18">
         <v>7</v>
@@ -5193,8 +4911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5204,94 +4922,94 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
-        <v>57</v>
-      </c>
       <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>72</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>73</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>74</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>75</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>76</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>77</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>79</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>80</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>81</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>82</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>83</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>84</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y1" t="s">
         <v>85</v>
       </c>
-      <c r="X1" t="s">
-        <v>150</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>86</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>87</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>88</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>89</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>90</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>91</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -5377,7 +5095,7 @@
         <v>0.08</v>
       </c>
       <c r="AE2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -5389,8 +5107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF59"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5400,97 +5118,97 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>96</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>97</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>98</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>99</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>100</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>101</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>102</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>103</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>104</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>105</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>106</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>107</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>108</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>109</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>110</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>111</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>112</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>113</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>114</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>115</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>116</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>117</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>118</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>119</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>120</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>121</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>122</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
@@ -5498,7 +5216,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C2">
         <v>201111</v>
@@ -5596,7 +5314,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C3">
         <v>201112</v>
@@ -5694,7 +5412,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4">
         <v>201201</v>
@@ -5792,7 +5510,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5">
         <v>201202</v>
@@ -5890,7 +5608,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6">
         <v>201203</v>
@@ -5988,7 +5706,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C7">
         <v>201204</v>
@@ -6086,7 +5804,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8">
         <v>201205</v>
@@ -6184,7 +5902,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9">
         <v>201206</v>
@@ -6282,7 +6000,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10">
         <v>201207</v>
@@ -6380,7 +6098,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C11">
         <v>201208</v>
@@ -6478,7 +6196,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12">
         <v>201209</v>
@@ -6576,7 +6294,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C13">
         <v>201210</v>
@@ -6674,7 +6392,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14">
         <v>201211</v>
@@ -6772,7 +6490,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15">
         <v>201212</v>
@@ -6870,7 +6588,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16">
         <v>201301</v>
@@ -6968,7 +6686,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C17">
         <v>201302</v>
@@ -7066,7 +6784,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18">
         <v>201303</v>
@@ -7164,7 +6882,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19">
         <v>201304</v>
@@ -7262,7 +6980,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C20">
         <v>201305</v>
@@ -7360,7 +7078,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21">
         <v>201306</v>
@@ -7458,7 +7176,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C22">
         <v>201307</v>
@@ -7556,7 +7274,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C23">
         <v>201308</v>
@@ -7654,7 +7372,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24">
         <v>201309</v>
@@ -7752,7 +7470,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C25">
         <v>201310</v>
@@ -7850,7 +7568,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C26">
         <v>201311</v>
@@ -7948,7 +7666,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C27">
         <v>201312</v>
@@ -8046,7 +7764,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C28">
         <v>201401</v>
@@ -8144,7 +7862,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29">
         <v>201402</v>
@@ -8242,7 +7960,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30">
         <v>201403</v>
@@ -8340,7 +8058,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C31">
         <v>201404</v>
@@ -8438,7 +8156,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C32">
         <v>201405</v>
@@ -8536,7 +8254,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33">
         <v>201406</v>
@@ -8634,7 +8352,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C34">
         <v>201407</v>
@@ -8732,7 +8450,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C35">
         <v>201408</v>
@@ -8830,7 +8548,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C36">
         <v>201409</v>
@@ -8928,7 +8646,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C37">
         <v>201410</v>
@@ -9026,7 +8744,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C38">
         <v>201411</v>
@@ -9124,7 +8842,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C39">
         <v>201412</v>
@@ -9222,7 +8940,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C40">
         <v>201501</v>
@@ -9320,7 +9038,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C41">
         <v>201502</v>
@@ -9418,7 +9136,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C42">
         <v>201503</v>
@@ -9516,7 +9234,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C43">
         <v>201504</v>
@@ -9614,7 +9332,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C44">
         <v>201505</v>
@@ -9712,7 +9430,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C45">
         <v>201506</v>
@@ -9810,7 +9528,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C46">
         <v>201507</v>
@@ -9908,7 +9626,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C47">
         <v>201508</v>
@@ -10006,7 +9724,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C48">
         <v>201509</v>
@@ -10104,7 +9822,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C49">
         <v>201510</v>
@@ -10202,7 +9920,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C50">
         <v>201511</v>
@@ -10300,7 +10018,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51">
         <v>201512</v>
@@ -10398,7 +10116,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C52">
         <v>201601</v>
@@ -10496,7 +10214,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C53">
         <v>201602</v>
@@ -10594,7 +10312,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C54">
         <v>201603</v>
@@ -10692,7 +10410,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C55">
         <v>201604</v>
@@ -10790,7 +10508,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C56">
         <v>201605</v>
@@ -10888,7 +10606,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C57">
         <v>201606</v>
@@ -10986,7 +10704,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C58">
         <v>201607</v>
@@ -11084,7 +10802,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C59">
         <v>201608</v>

</xml_diff>